<commit_message>
re-run some notebooks for more sequential reading
</commit_message>
<xml_diff>
--- a/Python/Result/total_rmse.xlsx
+++ b/Python/Result/total_rmse.xlsx
@@ -168,9 +168,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -181,6 +178,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -504,7 +504,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -522,7 +522,7 @@
       <c r="F2" s="1">
         <v>1.7484720269679E-2</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>1.7350999999999998E-2</v>
       </c>
       <c r="H2" s="1">
@@ -534,11 +534,11 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7"/>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3.8929510931406598E-2</v>
       </c>
       <c r="D3" s="1">
@@ -557,12 +557,12 @@
         <v>4.0132733038123203E-2</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J29" si="0">MIN(D3:H3)</f>
+        <f t="shared" ref="J3:J21" si="0">MIN(D3:H3)</f>
         <v>3.9459365088531401E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7"/>
       <c r="B4">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
       <c r="G4" s="1">
         <v>5.3834E-2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>5.1780755786365103E-2</v>
       </c>
       <c r="J4" s="1">
@@ -590,11 +590,11 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="7"/>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8.1540378555287896E-2</v>
       </c>
       <c r="D5" s="1">
@@ -618,13 +618,13 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>7.6060840277869602E-3</v>
       </c>
       <c r="D6" s="1">
@@ -648,11 +648,11 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="7"/>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1.82300820299145E-2</v>
       </c>
       <c r="D7" s="1">
@@ -676,11 +676,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="7"/>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2.95231217371082E-2</v>
       </c>
       <c r="D8" s="1">
@@ -704,11 +704,11 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="7"/>
       <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>4.58387867170661E-2</v>
       </c>
       <c r="D9" s="1">
@@ -732,7 +732,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -747,7 +747,7 @@
       <c r="E10" s="1">
         <v>2.0786501246190501E-2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>2.01115061988652E-2</v>
       </c>
       <c r="G10" s="1">
@@ -762,7 +762,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="7"/>
       <c r="B11">
         <v>3</v>
       </c>
@@ -781,7 +781,7 @@
       <c r="G11" s="1">
         <v>4.3734000000000002E-2</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>4.1430417531551897E-2</v>
       </c>
       <c r="J11" s="1">
@@ -790,11 +790,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="7"/>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>6.2737428493619296E-2</v>
       </c>
       <c r="D12" s="1">
@@ -818,11 +818,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="7"/>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>9.6898808521628799E-2</v>
       </c>
       <c r="D13" s="1">
@@ -846,7 +846,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -858,7 +858,7 @@
       <c r="D14" s="1">
         <v>2.19184340620662E-2</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>2.14684605934953E-2</v>
       </c>
       <c r="F14" s="1">
@@ -876,11 +876,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="7"/>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>4.4146811357768399E-2</v>
       </c>
       <c r="D15" s="1">
@@ -904,11 +904,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>6.5964758188812395E-2</v>
       </c>
       <c r="D16" s="1">
@@ -932,11 +932,11 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="7"/>
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>9.3917076070207897E-2</v>
       </c>
       <c r="D17" s="1">
@@ -960,7 +960,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B18">
@@ -975,7 +975,7 @@
       <c r="E18" s="1">
         <v>1.5316379138700599E-2</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>1.4854012086154E-2</v>
       </c>
       <c r="G18" s="1">
@@ -990,11 +990,11 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>3.1090792233025299E-2</v>
       </c>
       <c r="D19" s="1">
@@ -1018,11 +1018,11 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="7"/>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>3.88136614390081E-2</v>
       </c>
       <c r="D20" s="1">
@@ -1046,11 +1046,11 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="7"/>
       <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>4.7707293132415098E-2</v>
       </c>
       <c r="D21" s="1">
@@ -1074,7 +1074,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B22">
@@ -1086,7 +1086,7 @@
       <c r="D22" s="1">
         <v>1.78357718429209E-2</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>1.7093294226464498E-2</v>
       </c>
       <c r="F22" s="1">
@@ -1107,7 +1107,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="7"/>
       <c r="B23">
         <v>3</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="H23" s="1">
         <v>4.66063344408175E-2</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <v>3.2104000000000001E-2</v>
       </c>
       <c r="J23" s="1">
@@ -1138,7 +1138,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="7"/>
       <c r="B24">
         <v>6</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H24" s="1">
         <v>7.7624818485543895E-2</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <v>5.4436999999999999E-2</v>
       </c>
       <c r="J24" s="1">
@@ -1169,7 +1169,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="7"/>
       <c r="B25">
         <v>12</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H25" s="1">
         <v>0.13878832579581801</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <v>9.0106000000000006E-2</v>
       </c>
       <c r="J25" s="1">
@@ -1200,7 +1200,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B26">
@@ -1209,16 +1209,16 @@
       <c r="C26">
         <v>1.2458E-2</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2">
         <v>1.24877692311181E-2</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>6.03526527706468E-3</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F26" s="2">
         <v>7.8172052777944201E-3</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G26" s="2">
         <v>6.2196700997458297E-3</v>
       </c>
       <c r="H26">
@@ -1233,23 +1233,23 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="7"/>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27">
         <v>3.0086000000000002E-2</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>3.0678660077248902E-2</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>2.33674926133981E-2</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>2.66403559847735E-2</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>2.4510939693224602E-2</v>
       </c>
       <c r="H27">
@@ -1264,29 +1264,29 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="7"/>
       <c r="B28">
         <v>6</v>
       </c>
       <c r="C28">
         <v>4.6018000000000003E-2</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>4.70697002154584E-2</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>4.2968882233300601E-2</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>4.4412135891018098E-2</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>4.3285950120000499E-2</v>
       </c>
       <c r="H28">
         <v>8.0753127999999993E-2</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="4">
         <v>4.2299999999999997E-2</v>
       </c>
       <c r="J28" s="1">
@@ -1295,29 +1295,29 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="7"/>
       <c r="B29">
         <v>12</v>
       </c>
       <c r="C29">
         <v>5.5879999999999999E-2</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>5.4118306256134403E-2</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>5.8327282425377103E-2</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>5.70340619823154E-2</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>5.7471703768708998E-2</v>
       </c>
       <c r="H29">
         <v>0.114309507</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="4">
         <v>4.2897999999999999E-2</v>
       </c>
       <c r="J29" s="1">
@@ -1377,13 +1377,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1.84847659879337E-2</v>
       </c>
       <c r="D2">
@@ -1407,11 +1407,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7"/>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3.8929510931406598E-2</v>
       </c>
       <c r="D3">
@@ -1435,11 +1435,11 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7"/>
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>5.2929715994414102E-2</v>
       </c>
       <c r="D4">
@@ -1463,11 +1463,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="7"/>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8.1540378555287896E-2</v>
       </c>
       <c r="D5">
@@ -1491,13 +1491,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>7.6060840277869602E-3</v>
       </c>
       <c r="D6">
@@ -1518,11 +1518,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="7"/>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>1.82300820299145E-2</v>
       </c>
       <c r="D7">
@@ -1543,11 +1543,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="7"/>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>2.95231217371082E-2</v>
       </c>
       <c r="D8">
@@ -1568,11 +1568,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="7"/>
       <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>4.58387867170661E-2</v>
       </c>
       <c r="D9">
@@ -1593,13 +1593,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>2.10600365816512E-2</v>
       </c>
       <c r="D10">
@@ -1620,11 +1620,11 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="7"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>4.2205342153022601E-2</v>
       </c>
       <c r="D11">
@@ -1645,11 +1645,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="7"/>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>6.2737428493619296E-2</v>
       </c>
       <c r="D12">
@@ -1670,11 +1670,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="7"/>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>9.6898808521628799E-2</v>
       </c>
       <c r="D13">
@@ -1695,13 +1695,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>2.1630311969723801E-2</v>
       </c>
       <c r="D14">
@@ -1722,11 +1722,11 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="7"/>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>4.4146811357768399E-2</v>
       </c>
       <c r="D15">
@@ -1747,11 +1747,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>6.5964758188812395E-2</v>
       </c>
       <c r="D16">
@@ -1772,11 +1772,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="7"/>
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>9.3917076070207897E-2</v>
       </c>
       <c r="D17">
@@ -1797,7 +1797,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B18">
@@ -1812,7 +1812,7 @@
       <c r="E18">
         <v>2.1478580324699102E-2</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>1.5537E-2</v>
       </c>
       <c r="G18">
@@ -1824,7 +1824,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
       <c r="B19">
         <v>3</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="E19">
         <v>1.5855377441101299</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>2.7358E-2</v>
       </c>
       <c r="G19">
@@ -1849,7 +1849,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="7"/>
       <c r="B20">
         <v>6</v>
       </c>
@@ -1862,10 +1862,10 @@
       <c r="E20">
         <v>2.4999889009316298</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>3.0834E-2</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>3.0293E-2</v>
       </c>
       <c r="I20">
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="7"/>
       <c r="B21">
         <v>12</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="E21">
         <v>3.6985666061629998</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>3.4799999999999998E-2</v>
       </c>
       <c r="G21">
@@ -1899,13 +1899,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>1.7758748555011701E-2</v>
       </c>
       <c r="D22">
@@ -1926,11 +1926,11 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="7"/>
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>3.89252647151574E-2</v>
       </c>
       <c r="D23">
@@ -1951,11 +1951,11 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="7"/>
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>6.2944071349995898E-2</v>
       </c>
       <c r="D24">
@@ -1976,11 +1976,11 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="7"/>
       <c r="B25">
         <v>12</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>9.9058093819072601E-2</v>
       </c>
       <c r="D25">
@@ -2001,13 +2001,13 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>1.2458E-2</v>
       </c>
       <c r="D26">
@@ -2022,11 +2022,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="7"/>
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>3.0086000000000002E-2</v>
       </c>
       <c r="D27">
@@ -2041,11 +2041,11 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="7"/>
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>4.6018000000000003E-2</v>
       </c>
       <c r="D28">
@@ -2060,11 +2060,11 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="7"/>
       <c r="B29">
         <v>12</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>5.5879999999999999E-2</v>
       </c>
       <c r="D29">
@@ -2074,7 +2074,7 @@
         <v>5.5854000000000001E-2</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I3:I29" si="1">MIN(D29:G29)</f>
+        <f t="shared" ref="I29" si="1">MIN(D29:G29)</f>
         <v>5.5854000000000001E-2</v>
       </c>
     </row>
@@ -2097,8 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2127,7 +2127,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2">
@@ -2145,7 +2145,7 @@
       <c r="F2">
         <v>1.7478661121564602E-2</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>1.7149999999999999E-2</v>
       </c>
       <c r="H2">
@@ -2154,11 +2154,11 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7"/>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3.8929510931406598E-2</v>
       </c>
       <c r="D3">
@@ -2179,11 +2179,11 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7"/>
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>5.2929715994414102E-2</v>
       </c>
       <c r="D4">
@@ -2204,11 +2204,11 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="7"/>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8.1540378555287896E-2</v>
       </c>
       <c r="D5">
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6">
@@ -2244,7 +2244,7 @@
       <c r="E6">
         <v>7.4000000000000003E-3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>6.4270000000000004E-3</v>
       </c>
       <c r="G6">
@@ -2256,7 +2256,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="7"/>
       <c r="B7">
         <v>3</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="E7">
         <v>1.8305999999999999E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1.7069999999999998E-2</v>
       </c>
       <c r="G7">
@@ -2281,7 +2281,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="7"/>
       <c r="B8">
         <v>6</v>
       </c>
@@ -2297,7 +2297,7 @@
       <c r="F8">
         <v>2.9045000000000001E-2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>2.8674000000000002E-2</v>
       </c>
       <c r="H8">
@@ -2306,11 +2306,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="7"/>
       <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>4.58387867170661E-2</v>
       </c>
       <c r="D9">
@@ -2331,7 +2331,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -2340,7 +2340,7 @@
       <c r="C10">
         <v>2.10600365816512E-2</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>2.0105999999999999E-2</v>
       </c>
       <c r="E10">
@@ -2358,11 +2358,11 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="7"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>4.2205342153022601E-2</v>
       </c>
       <c r="D11">
@@ -2383,11 +2383,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="7"/>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>6.2737428493619296E-2</v>
       </c>
       <c r="D12">
@@ -2408,11 +2408,11 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="7"/>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>9.6898808521628799E-2</v>
       </c>
       <c r="D13">
@@ -2433,7 +2433,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B14">
@@ -2451,7 +2451,7 @@
       <c r="F14">
         <v>2.13696616394803E-2</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>2.1260635089413799E-2</v>
       </c>
       <c r="H14">
@@ -2460,11 +2460,11 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="7"/>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>4.4146811357768399E-2</v>
       </c>
       <c r="D15">
@@ -2485,11 +2485,11 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>6.5964758188812395E-2</v>
       </c>
       <c r="D16">
@@ -2510,11 +2510,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="7"/>
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>9.3917076070207897E-2</v>
       </c>
       <c r="D17">
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B18">
@@ -2553,7 +2553,7 @@
       <c r="F18">
         <v>1.5121537536553899E-2</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>1.4402E-2</v>
       </c>
       <c r="H18">
@@ -2562,7 +2562,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
       <c r="B19">
         <v>3</v>
       </c>
@@ -2578,7 +2578,7 @@
       <c r="F19">
         <v>3.39649722043633E-2</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>3.0287000000000001E-2</v>
       </c>
       <c r="H19">
@@ -2587,7 +2587,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="7"/>
       <c r="B20">
         <v>6</v>
       </c>
@@ -2597,7 +2597,7 @@
       <c r="D20">
         <v>4.1155999999999998E-2</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>3.6762000000000003E-2</v>
       </c>
       <c r="F20">
@@ -2612,11 +2612,11 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="7"/>
       <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>4.7707293132415098E-2</v>
       </c>
       <c r="D21">
@@ -2637,7 +2637,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B22">
@@ -2652,7 +2652,7 @@
       <c r="E22">
         <v>0.17706</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>1.7055000000000001E-2</v>
       </c>
       <c r="G22">
@@ -2664,7 +2664,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="7"/>
       <c r="B23">
         <v>3</v>
       </c>
@@ -2677,7 +2677,7 @@
       <c r="E23">
         <v>4.2820999999999998E-2</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>3.8482000000000002E-2</v>
       </c>
       <c r="G23">
@@ -2689,11 +2689,11 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="7"/>
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>6.2944071349995898E-2</v>
       </c>
       <c r="D24">
@@ -2714,11 +2714,11 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="7"/>
       <c r="B25">
         <v>12</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>9.9058093819072601E-2</v>
       </c>
       <c r="D25">
@@ -2739,7 +2739,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B26">
@@ -2757,7 +2757,7 @@
       <c r="F26">
         <v>1.0621999999999999E-2</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>1.0621999999999999E-2</v>
       </c>
       <c r="H26">
@@ -2766,7 +2766,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="7"/>
       <c r="B27">
         <v>3</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="E27">
         <v>2.9898000000000001E-2</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>2.9038999999999999E-2</v>
       </c>
       <c r="G27">
@@ -2791,11 +2791,11 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="7"/>
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>4.6018000000000003E-2</v>
       </c>
       <c r="D28">
@@ -2816,11 +2816,11 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="7"/>
       <c r="B29">
         <v>12</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>5.5879999999999999E-2</v>
       </c>
       <c r="D29">
@@ -2860,12 +2860,12 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2886,13 +2886,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>1.84847659879337E-2</v>
       </c>
       <c r="D2">
@@ -2901,7 +2901,7 @@
       <c r="E2">
         <v>1.9553999999999998E-2</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1.7149999999999999E-2</v>
       </c>
       <c r="G2">
@@ -2918,11 +2918,11 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
+      <c r="A3" s="7"/>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3.8929510931406598E-2</v>
       </c>
       <c r="D3">
@@ -2948,14 +2948,14 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="7"/>
       <c r="B4">
         <v>6</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>5.2929715994414102E-2</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5.1780755786365103E-2</v>
       </c>
       <c r="E4">
@@ -2978,11 +2978,11 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="7"/>
       <c r="B5">
         <v>12</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>8.1540378555287896E-2</v>
       </c>
       <c r="D5">
@@ -3008,13 +3008,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>7.6060840277869602E-3</v>
       </c>
       <c r="D6">
@@ -3023,7 +3023,7 @@
       <c r="E6">
         <v>7.8130000000000005E-3</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>6.4270000000000004E-3</v>
       </c>
       <c r="G6">
@@ -3034,17 +3034,17 @@
         <f t="shared" si="1"/>
         <v>6.4270000000000004E-3</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <f t="shared" si="2"/>
         <v>0.15501853824904718</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="7"/>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>1.82300820299145E-2</v>
       </c>
       <c r="D7">
@@ -3053,7 +3053,7 @@
       <c r="E7">
         <v>1.8727000000000001E-2</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>1.7069999999999998E-2</v>
       </c>
       <c r="G7">
@@ -3070,11 +3070,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="7"/>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>2.95231217371082E-2</v>
       </c>
       <c r="D8">
@@ -3083,7 +3083,7 @@
       <c r="E8">
         <v>2.9857999999999999E-2</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>2.8674000000000002E-2</v>
       </c>
       <c r="G8">
@@ -3100,11 +3100,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="7"/>
       <c r="B9">
         <v>12</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>4.58387867170661E-2</v>
       </c>
       <c r="D9">
@@ -3113,7 +3113,7 @@
       <c r="E9">
         <v>4.6341E-2</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>4.5686499999999998E-2</v>
       </c>
       <c r="G9">
@@ -3130,13 +3130,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>2.10600365816512E-2</v>
       </c>
       <c r="D10">
@@ -3145,7 +3145,7 @@
       <c r="E10">
         <v>2.1238507543531401E-2</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>2.0105999999999999E-2</v>
       </c>
       <c r="G10">
@@ -3162,14 +3162,14 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="7"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>4.2205342153022601E-2</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>4.1430417531551897E-2</v>
       </c>
       <c r="E11">
@@ -3192,11 +3192,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="7"/>
       <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>6.2737428493619296E-2</v>
       </c>
       <c r="D12">
@@ -3222,11 +3222,11 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="7"/>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>9.6898808521628799E-2</v>
       </c>
       <c r="D13">
@@ -3252,13 +3252,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>2.1630311969723801E-2</v>
       </c>
       <c r="D14">
@@ -3267,7 +3267,7 @@
       <c r="E14">
         <v>2.3227999999999999E-2</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>2.1260635089413799E-2</v>
       </c>
       <c r="G14">
@@ -3284,11 +3284,11 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="7"/>
       <c r="B15">
         <v>3</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>4.4146811357768399E-2</v>
       </c>
       <c r="D15">
@@ -3314,11 +3314,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
+      <c r="A16" s="7"/>
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>6.5964758188812395E-2</v>
       </c>
       <c r="D16">
@@ -3344,11 +3344,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
+      <c r="A17" s="7"/>
       <c r="B17">
         <v>12</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>9.3917076070207897E-2</v>
       </c>
       <c r="D17">
@@ -3374,13 +3374,13 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>1.5984916805093102E-2</v>
       </c>
       <c r="D18">
@@ -3389,7 +3389,7 @@
       <c r="E18">
         <v>1.5537E-2</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>1.4402E-2</v>
       </c>
       <c r="G18">
@@ -3400,23 +3400,23 @@
         <f t="shared" si="1"/>
         <v>1.4402E-2</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <f t="shared" si="2"/>
         <v>9.9025651768719497E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="7"/>
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>3.1090792233025299E-2</v>
       </c>
       <c r="D19">
         <v>3.1377754120751403E-2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>2.7358E-2</v>
       </c>
       <c r="F19">
@@ -3430,23 +3430,23 @@
         <f t="shared" si="1"/>
         <v>2.7358E-2</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <f t="shared" si="2"/>
         <v>0.12006102015825276</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
+      <c r="A20" s="7"/>
       <c r="B20">
         <v>6</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>3.88136614390081E-2</v>
       </c>
       <c r="D20">
         <v>3.8993E-2</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>3.0293E-2</v>
       </c>
       <c r="F20">
@@ -3460,23 +3460,23 @@
         <f t="shared" si="1"/>
         <v>3.0293E-2</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <f t="shared" si="2"/>
         <v>0.21952738090420795</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="A21" s="7"/>
       <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>4.7707293132415098E-2</v>
       </c>
       <c r="D21">
         <v>4.7939000000000002E-2</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>3.4799999999999998E-2</v>
       </c>
       <c r="F21">
@@ -3490,19 +3490,19 @@
         <f t="shared" si="1"/>
         <v>3.4799999999999998E-2</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <f t="shared" si="2"/>
         <v>0.2705517811834337</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>1.7758748555011701E-2</v>
       </c>
       <c r="D22">
@@ -3511,7 +3511,7 @@
       <c r="E22">
         <v>2.0523E-2</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>1.7055000000000001E-2</v>
       </c>
       <c r="G22">
@@ -3528,20 +3528,20 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
+      <c r="A23" s="7"/>
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6">
         <v>3.89252647151574E-2</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>3.2104000000000001E-2</v>
       </c>
       <c r="E23">
         <v>4.5865999999999997E-2</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>3.8482000000000002E-2</v>
       </c>
       <c r="G23">
@@ -3552,20 +3552,20 @@
         <f t="shared" si="1"/>
         <v>3.2104000000000001E-2</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <f t="shared" si="2"/>
         <v>0.17524003407743599</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
+      <c r="A24" s="7"/>
       <c r="B24">
         <v>6</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6">
         <v>6.2944071349995898E-2</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>5.4436999999999999E-2</v>
       </c>
       <c r="E24">
@@ -3582,20 +3582,20 @@
         <f t="shared" si="1"/>
         <v>5.4436999999999999E-2</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <f t="shared" si="2"/>
         <v>0.13515286138217769</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
+      <c r="A25" s="7"/>
       <c r="B25">
         <v>12</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>9.9058093819072601E-2</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>9.0106000000000006E-2</v>
       </c>
       <c r="E25">
@@ -3618,7 +3618,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B26">
@@ -3627,7 +3627,7 @@
       <c r="C26">
         <v>1.2458E-2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>6.03526527706468E-3</v>
       </c>
       <c r="E26">
@@ -3644,20 +3644,20 @@
         <f t="shared" si="1"/>
         <v>6.03526527706468E-3</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <f t="shared" si="2"/>
         <v>0.51555102929325092</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
+      <c r="A27" s="7"/>
       <c r="B27">
         <v>3</v>
       </c>
       <c r="C27">
         <v>3.0086000000000002E-2</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <v>2.33674926133981E-2</v>
       </c>
       <c r="E27">
@@ -3674,20 +3674,20 @@
         <f t="shared" si="1"/>
         <v>2.33674926133981E-2</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="4">
         <f t="shared" si="2"/>
         <v>0.22331009062693283</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
+      <c r="A28" s="7"/>
       <c r="B28">
         <v>6</v>
       </c>
       <c r="C28">
         <v>4.6018000000000003E-2</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>4.2299999999999997E-2</v>
       </c>
       <c r="E28">
@@ -3710,14 +3710,14 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
+      <c r="A29" s="7"/>
       <c r="B29">
         <v>12</v>
       </c>
       <c r="C29">
         <v>5.5879999999999999E-2</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>4.2897999999999999E-2</v>
       </c>
       <c r="E29">
@@ -3734,7 +3734,7 @@
         <f t="shared" si="1"/>
         <v>4.2897999999999999E-2</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="4">
         <f t="shared" si="2"/>
         <v>0.23231925554760202</v>
       </c>

</xml_diff>